<commit_message>
Added my ppt work
</commit_message>
<xml_diff>
--- a/Work.xlsx
+++ b/Work.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yash Tripathi\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="96" yWindow="72" windowWidth="9492" windowHeight="6336"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Anmol Shukla</t>
   </si>
@@ -57,26 +62,35 @@
     <t>24th Feb</t>
   </si>
   <si>
-    <t>20min</t>
-  </si>
-  <si>
-    <t>60min</t>
-  </si>
-  <si>
     <t>missing</t>
   </si>
   <si>
-    <t>75min</t>
-  </si>
-  <si>
     <t>Remarks</t>
+  </si>
+  <si>
+    <t>28th Feb</t>
+  </si>
+  <si>
+    <t>15min</t>
+  </si>
+  <si>
+    <t>90min</t>
+  </si>
+  <si>
+    <t>30min</t>
+  </si>
+  <si>
+    <t>Started PPT</t>
+  </si>
+  <si>
+    <t>75% PPT completed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,17 +132,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -136,6 +150,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -182,7 +204,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -214,9 +236,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -248,6 +271,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -423,53 +447,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="F6" sqref="F6:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
     </row>
-    <row r="2" spans="1:23">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="4"/>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
@@ -477,9 +503,11 @@
         <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -498,11 +526,11 @@
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
     </row>
-    <row r="3" spans="1:23">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
@@ -510,9 +538,11 @@
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -531,11 +561,11 @@
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
     </row>
-    <row r="4" spans="1:23">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
@@ -543,9 +573,11 @@
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -564,11 +596,11 @@
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
     </row>
-    <row r="5" spans="1:23">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
@@ -578,7 +610,9 @@
       <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -597,77 +631,84 @@
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
     </row>
-    <row r="6" spans="1:23">
-      <c r="A6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5" t="s">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-    </row>
-    <row r="7" spans="1:23">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:23">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:23">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:23">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+      <c r="E6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:B3"/>
     <mergeCell ref="F6:F10"/>
     <mergeCell ref="G6:G10"/>
     <mergeCell ref="H6:H10"/>
@@ -677,9 +718,6 @@
     <mergeCell ref="C6:C10"/>
     <mergeCell ref="D6:D10"/>
     <mergeCell ref="E6:E10"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -687,24 +725,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>